<commit_message>
Update ideas video michelina
</commit_message>
<xml_diff>
--- a/German/Clase 13/Performance exp colaborativos (clase 13).xlsx
+++ b/German/Clase 13/Performance exp colaborativos (clase 13).xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\German\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\German\Desktop\dmeyf2023\German\Clase 13\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3A47410-6E11-4233-8D46-7D8AE9623A6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B68E76C-31E5-439D-BB52-0DC071124E9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Fechas del Experimento" sheetId="6" r:id="rId1"/>
@@ -1520,6 +1520,12 @@
     <xf numFmtId="0" fontId="2" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1571,9 +1577,6 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1583,11 +1586,8 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2234,6 +2234,987 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US" sz="1050" baseline="0"/>
+              <a:t>Semilla 2 (279523)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1050"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.21512027854861052"/>
+          <c:y val="0"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-AR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.16999847082065808"/>
+          <c:y val="0.11152777777777778"/>
+          <c:w val="0.81888501232377531"/>
+          <c:h val="0.60190039536197204"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Ganancia por Iteración'!$B$1:$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Modelo Base</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="002060"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Ganancia por Iteración'!$A$3:$A$68</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="66"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>61</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>66</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Ganancia por Iteración'!$C$4:$C$68</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="65"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-455A-4CDF-8E1F-FF63FA55B967}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Ganancia por Iteración'!#REF!</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>#REF!</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Ganancia por Iteración'!$A$3:$A$68</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="66"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>61</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>66</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Ganancia por Iteración'!#REF!</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-455A-4CDF-8E1F-FF63FA55B967}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="942592416"/>
+        <c:axId val="11533312"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="942592416"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-AR"/>
+                  <a:t>Estímulos</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-AR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-AR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="11533312"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="11533312"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="110000000000000.02"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-AR"/>
+                  <a:t>Ganancia Test (millones)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="3.2258192457135601E-4"/>
+              <c:y val="0.33001993421708364"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-AR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="#,##0" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-AR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="942592416"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:dispUnits>
+          <c:builtInUnit val="billions"/>
+        </c:dispUnits>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0"/>
+          <c:y val="0.87691949898667731"/>
+          <c:w val="1"/>
+          <c:h val="0.12267151732615701"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-AR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-AR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1050"/>
+              <a:t>Ganancia de BO </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1050" baseline="0"/>
+              <a:t>de LGBM en Jul-21 en 66 iteraciones:</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1050"/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1050" baseline="0"/>
               <a:t>Semilla 4 (279551)</a:t>
             </a:r>
           </a:p>
@@ -3172,7 +4153,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="es-ES"/>
@@ -7642,7 +8623,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US" sz="1050"/>
-              <a:t>Promedio 6 semillas score</a:t>
+              <a:t>Promedio 5 semillas score</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" sz="1050" baseline="0"/>
@@ -8222,22 +9203,20 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US" sz="1050"/>
-              <a:t>Ganancia de BO </a:t>
+              <a:t>Promedio 5 semillas Score</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" sz="1050" baseline="0"/>
-              <a:t>de LGBM en Jul-21 en 66 iteraciones:</a:t>
+              <a:t> Observado en Sep-21y </a:t>
             </a:r>
-          </a:p>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1050"/>
-            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1050"/>
+              <a:t>Cantidad</a:t>
+            </a:r>
             <a:r>
               <a:rPr lang="en-US" sz="1050" baseline="0"/>
-              <a:t>Semilla 1 (279511)</a:t>
+              <a:t> de Estímulos Enviados</a:t>
             </a:r>
-            <a:endParaRPr lang="en-US" sz="1050"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -8245,7 +9224,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.21512027854861052"/>
+          <c:x val="0.12826880107635755"/>
           <c:y val="0"/>
         </c:manualLayout>
       </c:layout>
@@ -8285,10 +9264,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.16999847082065808"/>
-          <c:y val="0.11152777777777778"/>
-          <c:w val="0.81888501232377531"/>
-          <c:h val="0.60190039536197204"/>
+          <c:x val="0.13261976594257369"/>
+          <c:y val="0.16009645135821438"/>
+          <c:w val="0.843202518365465"/>
+          <c:h val="0.60225038943302822"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -8299,11 +9278,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Ganancia por Iteración'!$B$1:$G$1</c:f>
+              <c:f>'Semill búsqueda de la meseta'!$L$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Modelo Base</c:v>
+                  <c:v>Promedio 5 bos</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -8336,488 +9315,98 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Ganancia por Iteración'!$A$3:$A$68</c:f>
+              <c:f>'Semill búsqueda de la meseta'!$A$4:$A$15</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="66"/>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>8000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>8500</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>9000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4</c:v>
+                  <c:v>9500</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5</c:v>
+                  <c:v>10000</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6</c:v>
+                  <c:v>10500</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7</c:v>
+                  <c:v>11000</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8</c:v>
+                  <c:v>11500</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9</c:v>
+                  <c:v>12000</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>10</c:v>
+                  <c:v>12500</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>11</c:v>
+                  <c:v>13000</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>23</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>26</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>27</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>28</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>29</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>31</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>33</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>34</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>35</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>36</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>37</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>38</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>39</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>41</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>42</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>43</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>44</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>45</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>46</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>47</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>48</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>49</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>51</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>52</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>53</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>54</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>55</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>56</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>57</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>58</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>59</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>60</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>61</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>62</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>63</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>64</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>65</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>66</c:v>
+                  <c:v>13500</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Ganancia por Iteración'!$B$4:$B$68</c:f>
+              <c:f>'Semill búsqueda de la meseta'!$L$4:$L$15</c:f>
               <c:numCache>
-                <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="65"/>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>114.07620000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>117.7864</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>122.60299999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>124.74480000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>125.71080000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>124.255</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>122.477</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>121.8468</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>118.5146</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>118.58459999999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>116.2882</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>114.5522</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-E220-4C17-A585-79E590329065}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Ganancia por Iteración'!#REF!</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>#REF!</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>'Ganancia por Iteración'!$A$3:$A$68</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="66"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>23</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>26</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>27</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>28</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>29</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>31</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>33</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>34</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>35</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>36</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>37</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>38</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>39</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>41</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>42</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>43</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>44</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>45</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>46</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>47</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>48</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>49</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>51</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>52</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>53</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>54</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>55</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>56</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>57</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>58</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>59</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>60</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>61</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>62</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>63</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>64</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>65</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>66</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Ganancia por Iteración'!#REF!</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-E220-4C17-A585-79E590329065}"/>
+              <c16:uniqueId val="{00000000-D8DC-42F5-8C30-D69B3A6770BA}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -8910,7 +9499,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="#,##0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -8958,7 +9547,7 @@
         <c:axId val="11533312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="110000000000000.02"/>
+          <c:min val="110"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -8997,19 +9586,11 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="es-AR"/>
-                  <a:t>Ganancia Test (millones)</a:t>
+                  <a:t>Score Observado</a:t>
                 </a:r>
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout>
-            <c:manualLayout>
-              <c:xMode val="edge"/>
-              <c:yMode val="edge"/>
-              <c:x val="3.2258192457135601E-4"/>
-              <c:y val="0.33001993421708364"/>
-            </c:manualLayout>
-          </c:layout>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -9073,9 +9654,6 @@
         <c:crossAx val="942592416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
-        <c:dispUnits>
-          <c:builtInUnit val="billions"/>
-        </c:dispUnits>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -9085,47 +9663,6 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout>
-        <c:manualLayout>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0"/>
-          <c:y val="0.87691949898667731"/>
-          <c:w val="1"/>
-          <c:h val="0.12267151732615701"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="es-AR"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -9218,7 +9755,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US" sz="1050" baseline="0"/>
-              <a:t>Semilla 2 (279523)</a:t>
+              <a:t>Semilla 1 (279511)</a:t>
             </a:r>
             <a:endParaRPr lang="en-US" sz="1050"/>
           </a:p>
@@ -9310,7 +9847,9 @@
                 </a:schemeClr>
               </a:solidFill>
               <a:ln w="9525">
-                <a:noFill/>
+                <a:solidFill>
+                  <a:srgbClr val="002060"/>
+                </a:solidFill>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
@@ -9524,7 +10063,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Ganancia por Iteración'!$C$4:$C$68</c:f>
+              <c:f>'Ganancia por Iteración'!$B$4:$B$68</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="65"/>
@@ -9534,7 +10073,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-455A-4CDF-8E1F-FF63FA55B967}"/>
+              <c16:uniqueId val="{00000000-E220-4C17-A585-79E590329065}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -9798,7 +10337,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-455A-4CDF-8E1F-FF63FA55B967}"/>
+              <c16:uniqueId val="{00000001-E220-4C17-A585-79E590329065}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -10271,6 +10810,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors12.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -12139,6 +12718,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style12.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -16500,15 +17595,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>212912</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>145677</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>339437</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:colOff>552349</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>12327</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -16530,6 +17625,44 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>717176</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>22412</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>403412</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>56029</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Gráfico 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{72FE0AE6-623A-4E15-B56D-311552C80B6F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -16979,86 +18112,86 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="55" t="s">
+      <c r="A1" s="57" t="s">
         <v>115</v>
       </c>
-      <c r="B1" s="55"/>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
-      <c r="F1" s="55"/>
-      <c r="G1" s="55"/>
-      <c r="H1" s="55"/>
-      <c r="I1" s="55"/>
-      <c r="J1" s="55"/>
-      <c r="K1" s="55"/>
-      <c r="L1" s="55"/>
-      <c r="M1" s="55"/>
-      <c r="N1" s="55"/>
-      <c r="O1" s="55"/>
-      <c r="P1" s="55"/>
-      <c r="Q1" s="55"/>
-      <c r="R1" s="55"/>
-      <c r="S1" s="55"/>
-      <c r="T1" s="55"/>
-      <c r="U1" s="55"/>
-      <c r="V1" s="55"/>
-      <c r="W1" s="55"/>
-      <c r="X1" s="55"/>
-      <c r="Y1" s="55"/>
-      <c r="Z1" s="55"/>
-      <c r="AA1" s="55"/>
-      <c r="AB1" s="55"/>
-      <c r="AC1" s="55"/>
-      <c r="AD1" s="55"/>
-      <c r="AE1" s="55"/>
-      <c r="AF1" s="55"/>
-      <c r="AG1" s="55"/>
-      <c r="AH1" s="55"/>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="57"/>
+      <c r="K1" s="57"/>
+      <c r="L1" s="57"/>
+      <c r="M1" s="57"/>
+      <c r="N1" s="57"/>
+      <c r="O1" s="57"/>
+      <c r="P1" s="57"/>
+      <c r="Q1" s="57"/>
+      <c r="R1" s="57"/>
+      <c r="S1" s="57"/>
+      <c r="T1" s="57"/>
+      <c r="U1" s="57"/>
+      <c r="V1" s="57"/>
+      <c r="W1" s="57"/>
+      <c r="X1" s="57"/>
+      <c r="Y1" s="57"/>
+      <c r="Z1" s="57"/>
+      <c r="AA1" s="57"/>
+      <c r="AB1" s="57"/>
+      <c r="AC1" s="57"/>
+      <c r="AD1" s="57"/>
+      <c r="AE1" s="57"/>
+      <c r="AF1" s="57"/>
+      <c r="AG1" s="57"/>
+      <c r="AH1" s="57"/>
     </row>
     <row r="2" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A2" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="56">
+      <c r="B2" s="58">
         <v>2019</v>
       </c>
-      <c r="C2" s="57"/>
-      <c r="D2" s="57"/>
-      <c r="E2" s="57"/>
-      <c r="F2" s="57"/>
-      <c r="G2" s="57"/>
-      <c r="H2" s="57"/>
-      <c r="I2" s="57"/>
-      <c r="J2" s="57"/>
-      <c r="K2" s="57"/>
-      <c r="L2" s="57"/>
-      <c r="M2" s="58"/>
-      <c r="N2" s="56">
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="59"/>
+      <c r="F2" s="59"/>
+      <c r="G2" s="59"/>
+      <c r="H2" s="59"/>
+      <c r="I2" s="59"/>
+      <c r="J2" s="59"/>
+      <c r="K2" s="59"/>
+      <c r="L2" s="59"/>
+      <c r="M2" s="60"/>
+      <c r="N2" s="58">
         <v>2020</v>
       </c>
-      <c r="O2" s="57"/>
-      <c r="P2" s="57"/>
-      <c r="Q2" s="57"/>
-      <c r="R2" s="57"/>
-      <c r="S2" s="57"/>
-      <c r="T2" s="57"/>
-      <c r="U2" s="57"/>
-      <c r="V2" s="57"/>
-      <c r="W2" s="57"/>
-      <c r="X2" s="57"/>
-      <c r="Y2" s="58"/>
-      <c r="Z2" s="59">
+      <c r="O2" s="59"/>
+      <c r="P2" s="59"/>
+      <c r="Q2" s="59"/>
+      <c r="R2" s="59"/>
+      <c r="S2" s="59"/>
+      <c r="T2" s="59"/>
+      <c r="U2" s="59"/>
+      <c r="V2" s="59"/>
+      <c r="W2" s="59"/>
+      <c r="X2" s="59"/>
+      <c r="Y2" s="60"/>
+      <c r="Z2" s="61">
         <v>2021</v>
       </c>
-      <c r="AA2" s="60"/>
-      <c r="AB2" s="60"/>
-      <c r="AC2" s="60"/>
-      <c r="AD2" s="60"/>
-      <c r="AE2" s="60"/>
-      <c r="AF2" s="60"/>
-      <c r="AG2" s="60"/>
-      <c r="AH2" s="61"/>
+      <c r="AA2" s="62"/>
+      <c r="AB2" s="62"/>
+      <c r="AC2" s="62"/>
+      <c r="AD2" s="62"/>
+      <c r="AE2" s="62"/>
+      <c r="AF2" s="62"/>
+      <c r="AG2" s="62"/>
+      <c r="AH2" s="63"/>
     </row>
     <row r="3" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A3" s="36" t="s">
@@ -17210,13 +18343,13 @@
       <c r="O4" s="42">
         <v>1</v>
       </c>
-      <c r="P4" s="62" t="s">
+      <c r="P4" s="64" t="s">
         <v>118</v>
       </c>
-      <c r="Q4" s="63"/>
-      <c r="R4" s="63"/>
-      <c r="S4" s="63"/>
-      <c r="T4" s="64"/>
+      <c r="Q4" s="65"/>
+      <c r="R4" s="65"/>
+      <c r="S4" s="65"/>
+      <c r="T4" s="66"/>
       <c r="U4" s="42">
         <v>1</v>
       </c>
@@ -17270,11 +18403,11 @@
       <c r="M5" s="11"/>
       <c r="N5" s="10"/>
       <c r="O5" s="6"/>
-      <c r="P5" s="65"/>
-      <c r="Q5" s="66"/>
-      <c r="R5" s="66"/>
-      <c r="S5" s="66"/>
-      <c r="T5" s="67"/>
+      <c r="P5" s="67"/>
+      <c r="Q5" s="68"/>
+      <c r="R5" s="68"/>
+      <c r="S5" s="68"/>
+      <c r="T5" s="69"/>
       <c r="U5" s="6"/>
       <c r="V5" s="6"/>
       <c r="W5" s="6"/>
@@ -17310,11 +18443,11 @@
       <c r="M6" s="11"/>
       <c r="N6" s="10"/>
       <c r="O6" s="6"/>
-      <c r="P6" s="65"/>
-      <c r="Q6" s="66"/>
-      <c r="R6" s="66"/>
-      <c r="S6" s="66"/>
-      <c r="T6" s="67"/>
+      <c r="P6" s="67"/>
+      <c r="Q6" s="68"/>
+      <c r="R6" s="68"/>
+      <c r="S6" s="68"/>
+      <c r="T6" s="69"/>
       <c r="U6" s="6"/>
       <c r="V6" s="6"/>
       <c r="W6" s="6"/>
@@ -17374,11 +18507,11 @@
       <c r="O7" s="42">
         <v>1</v>
       </c>
-      <c r="P7" s="65"/>
-      <c r="Q7" s="66"/>
-      <c r="R7" s="66"/>
-      <c r="S7" s="66"/>
-      <c r="T7" s="67"/>
+      <c r="P7" s="67"/>
+      <c r="Q7" s="68"/>
+      <c r="R7" s="68"/>
+      <c r="S7" s="68"/>
+      <c r="T7" s="69"/>
       <c r="U7" s="42">
         <v>1</v>
       </c>
@@ -17436,11 +18569,11 @@
       <c r="M8" s="14"/>
       <c r="N8" s="12"/>
       <c r="O8" s="13"/>
-      <c r="P8" s="68"/>
-      <c r="Q8" s="69"/>
-      <c r="R8" s="69"/>
-      <c r="S8" s="69"/>
-      <c r="T8" s="70"/>
+      <c r="P8" s="70"/>
+      <c r="Q8" s="71"/>
+      <c r="R8" s="71"/>
+      <c r="S8" s="71"/>
+      <c r="T8" s="72"/>
       <c r="U8" s="13"/>
       <c r="V8" s="13"/>
       <c r="W8" s="13"/>
@@ -17512,12 +18645,12 @@
   </sheetPr>
   <dimension ref="A1:L34"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="L10" activePane="bottomRight" state="frozen"/>
       <selection activeCell="E8" sqref="E8"/>
       <selection pane="topRight" activeCell="E8" sqref="E8"/>
       <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
-      <selection pane="bottomRight" activeCell="J7" sqref="J7"/>
+      <selection pane="bottomRight" activeCell="Z19" sqref="Z19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17538,17 +18671,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B1" s="71" t="s">
+      <c r="B1" s="73" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="71"/>
-      <c r="D1" s="71"/>
-      <c r="E1" s="71"/>
-      <c r="F1" s="71"/>
-      <c r="G1" s="71"/>
-      <c r="H1" s="71"/>
-      <c r="I1" s="71"/>
-      <c r="J1" s="71"/>
+      <c r="C1" s="73"/>
+      <c r="D1" s="73"/>
+      <c r="E1" s="73"/>
+      <c r="F1" s="73"/>
+      <c r="G1" s="73"/>
+      <c r="H1" s="73"/>
+      <c r="I1" s="73"/>
+      <c r="J1" s="73"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B2" s="51" t="s">
@@ -18030,7 +19163,7 @@
   </sheetPr>
   <dimension ref="A1:L23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
@@ -18049,26 +19182,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="75" t="s">
+      <c r="A1" s="76" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="75"/>
-      <c r="C1" s="75"/>
-      <c r="D1" s="75"/>
-      <c r="E1" s="75"/>
-      <c r="F1" s="75"/>
-      <c r="G1" s="75"/>
+      <c r="B1" s="76"/>
+      <c r="C1" s="76"/>
+      <c r="D1" s="76"/>
+      <c r="E1" s="76"/>
+      <c r="F1" s="76"/>
+      <c r="G1" s="76"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="74" t="s">
+      <c r="A3" s="75" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="74"/>
-      <c r="C3" s="74"/>
-      <c r="D3" s="74"/>
-      <c r="E3" s="74"/>
-      <c r="F3" s="74"/>
-      <c r="G3" s="74"/>
+      <c r="B3" s="75"/>
+      <c r="C3" s="75"/>
+      <c r="D3" s="75"/>
+      <c r="E3" s="75"/>
+      <c r="F3" s="75"/>
+      <c r="G3" s="75"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
@@ -18216,7 +19349,7 @@
         <f t="shared" si="0"/>
         <v>124.74480000000001</v>
       </c>
-      <c r="I8" s="77" t="s">
+      <c r="I8" s="56" t="s">
         <v>298</v>
       </c>
       <c r="L8" s="5"/>
@@ -18238,7 +19371,7 @@
         <f>+'Semill búsqueda de la meseta'!F8</f>
         <v>126.355</v>
       </c>
-      <c r="E9" s="76">
+      <c r="E9" s="55">
         <f>+'Semill búsqueda de la meseta'!H8</f>
         <v>129.715</v>
       </c>
@@ -18461,15 +19594,15 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="73" t="s">
+      <c r="A17" s="74" t="s">
         <v>108</v>
       </c>
-      <c r="B17" s="73"/>
-      <c r="C17" s="73"/>
-      <c r="D17" s="73"/>
-      <c r="E17" s="73"/>
-      <c r="F17" s="73"/>
-      <c r="G17" s="73"/>
+      <c r="B17" s="74"/>
+      <c r="C17" s="74"/>
+      <c r="D17" s="74"/>
+      <c r="E17" s="74"/>
+      <c r="F17" s="74"/>
+      <c r="G17" s="74"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="16" t="s">
@@ -18649,14 +19782,14 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="25"/>
-      <c r="B1" s="72" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="72"/>
-      <c r="D1" s="72"/>
-      <c r="E1" s="72"/>
-      <c r="F1" s="72"/>
-      <c r="G1" s="72"/>
+      <c r="B1" s="77" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
       <c r="H1" s="27"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>